<commit_message>
corrected model with 3 scenarios.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="costs" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="utilities" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="strategy_params" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="screening_strategies" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>ParameterName</t>
   </si>
@@ -215,6 +216,48 @@
   </si>
   <si>
     <t>Year to use from the mortality file</t>
+  </si>
+  <si>
+    <t>screening_3_cost</t>
+  </si>
+  <si>
+    <t>Cost of 3 Pap tests ($8 each)</t>
+  </si>
+  <si>
+    <t>screening_10_cost</t>
+  </si>
+  <si>
+    <t>Cost of 10 Pap tests ($8 each)</t>
+  </si>
+  <si>
+    <t>screening_3_utility</t>
+  </si>
+  <si>
+    <t>Utility during Pap test year (3 tests)</t>
+  </si>
+  <si>
+    <t>screening_10_utility</t>
+  </si>
+  <si>
+    <t>Utility during Pap test year (10 tests)</t>
+  </si>
+  <si>
+    <t>screening_age_start</t>
+  </si>
+  <si>
+    <t>Age when screening begins</t>
+  </si>
+  <si>
+    <t>screening_3_freq</t>
+  </si>
+  <si>
+    <t>Number of screenings in 3-test strategy</t>
+  </si>
+  <si>
+    <t>screening_10_freq</t>
+  </si>
+  <si>
+    <t>Number of screenings in 10-test strategy</t>
   </si>
 </sst>
 </file>
@@ -276,6 +319,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1025,4 +1072,114 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.13"/>
+    <col customWidth="1" min="3" max="3" width="31.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>